<commit_message>
--- Published Release V1.7 ---
</commit_message>
<xml_diff>
--- a/IntegrationTool.UnitTests.Sources/TestData/LoadFromExcel/TestData.xlsx
+++ b/IntegrationTool.UnitTests.Sources/TestData/LoadFromExcel/TestData.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
   <si>
     <t>Firstname</t>
   </si>
@@ -140,6 +140,12 @@
   </si>
   <si>
     <t>ToLong To Long ToLong To Long ToLong To Long ToLong To Long ToLong To Long ToLong To Long ToLong To Long ToLong To Long ToLong To Long ToLong To Long</t>
+  </si>
+  <si>
+    <t>Birthd</t>
+  </si>
+  <si>
+    <t>10.02.1989</t>
   </si>
 </sst>
 </file>
@@ -182,9 +188,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -477,9 +485,10 @@
     <col min="2" max="2" width="141.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15">
+    <row r="1" spans="1:6" ht="15">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -495,8 +504,11 @@
       <c r="E1" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -512,8 +524,11 @@
       <c r="E2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="2">
+        <v>36932</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -529,8 +544,11 @@
       <c r="E3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="2">
+        <v>32843</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
@@ -541,7 +559,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
@@ -557,8 +575,11 @@
       <c r="E5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>5</v>
       </c>
@@ -568,6 +589,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Working on marketinglist target.
</commit_message>
<xml_diff>
--- a/IntegrationTool.UnitTests.Sources/TestData/LoadFromExcel/TestData.xlsx
+++ b/IntegrationTool.UnitTests.Sources/TestData/LoadFromExcel/TestData.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14250"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14250" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="1" r:id="rId1"/>
-    <sheet name="Accounts" sheetId="2" r:id="rId2"/>
-    <sheet name="Activities" sheetId="3" r:id="rId3"/>
+    <sheet name="Marketinglist" sheetId="4" r:id="rId2"/>
+    <sheet name="Accounts" sheetId="2" r:id="rId3"/>
+    <sheet name="Activities" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="44">
   <si>
     <t>Firstname</t>
   </si>
@@ -146,6 +147,18 @@
   </si>
   <si>
     <t>10.02.1989</t>
+  </si>
+  <si>
+    <t>My List 1</t>
+  </si>
+  <si>
+    <t>My List 2</t>
+  </si>
+  <si>
+    <t>My List 3</t>
+  </si>
+  <si>
+    <t>My Marketinglists</t>
   </si>
 </sst>
 </file>
@@ -475,7 +488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -594,6 +607,103 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="16.25" customWidth="1"/>
+    <col min="2" max="2" width="12.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15">
+      <c r="A1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -676,7 +786,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>

</xml_diff>

<commit_message>
Worked on marketinglist target. Soon ready to release!
</commit_message>
<xml_diff>
--- a/IntegrationTool.UnitTests.Sources/TestData/LoadFromExcel/TestData.xlsx
+++ b/IntegrationTool.UnitTests.Sources/TestData/LoadFromExcel/TestData.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14250" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14250" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="1" r:id="rId1"/>
     <sheet name="Marketinglist" sheetId="4" r:id="rId2"/>
-    <sheet name="Accounts" sheetId="2" r:id="rId3"/>
-    <sheet name="Activities" sheetId="3" r:id="rId4"/>
+    <sheet name="ManualMarketinglist" sheetId="5" r:id="rId3"/>
+    <sheet name="Accounts" sheetId="2" r:id="rId4"/>
+    <sheet name="Activities" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="44">
   <si>
     <t>Firstname</t>
   </si>
@@ -610,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -704,6 +705,53 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -786,7 +834,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>

</xml_diff>

<commit_message>
Wrote an additional test for incidents
</commit_message>
<xml_diff>
--- a/IntegrationTool.UnitTests.Sources/TestData/LoadFromExcel/TestData.xlsx
+++ b/IntegrationTool.UnitTests.Sources/TestData/LoadFromExcel/TestData.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14250" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14250" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="1" r:id="rId1"/>
     <sheet name="Marketinglist" sheetId="4" r:id="rId2"/>
     <sheet name="ManualMarketinglist" sheetId="5" r:id="rId3"/>
-    <sheet name="Accounts" sheetId="2" r:id="rId4"/>
-    <sheet name="Activities" sheetId="3" r:id="rId5"/>
+    <sheet name="Incidents" sheetId="6" r:id="rId4"/>
+    <sheet name="Accounts" sheetId="2" r:id="rId5"/>
+    <sheet name="Activities" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="49">
   <si>
     <t>Firstname</t>
   </si>
@@ -160,6 +161,21 @@
   </si>
   <si>
     <t>My Marketinglists</t>
+  </si>
+  <si>
+    <t>CaseId</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>My Case</t>
+  </si>
+  <si>
+    <t>Another Case</t>
+  </si>
+  <si>
+    <t>Company</t>
   </si>
 </sst>
 </file>
@@ -708,7 +724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -753,10 +769,62 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="2" max="2" width="19.125" customWidth="1"/>
+    <col min="3" max="3" width="20.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>123</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>456</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -834,7 +902,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>

</xml_diff>

<commit_message>
Fixed bug (multiple relations of the same type)
</commit_message>
<xml_diff>
--- a/IntegrationTool.UnitTests.Sources/TestData/LoadFromExcel/TestData.xlsx
+++ b/IntegrationTool.UnitTests.Sources/TestData/LoadFromExcel/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14250" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14250" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="51">
   <si>
     <t>Firstname</t>
   </si>
@@ -176,13 +176,19 @@
   </si>
   <si>
     <t>Company</t>
+  </si>
+  <si>
+    <t>OwnerId</t>
+  </si>
+  <si>
+    <t>CD723ABA-3C05-E411-89D3-000C29571E8B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -509,16 +515,16 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="141.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="141.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -538,7 +544,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -558,7 +564,7 @@
         <v>36932</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -578,7 +584,7 @@
         <v>32843</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -589,7 +595,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -609,7 +615,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -631,13 +637,13 @@
       <selection activeCell="B1" sqref="B1:C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.25" customWidth="1"/>
-    <col min="2" max="2" width="12.625" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>43</v>
       </c>
@@ -648,7 +654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -659,7 +665,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -670,7 +676,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -681,7 +687,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -692,7 +698,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -703,7 +709,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -728,9 +734,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="15">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -738,7 +744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -746,7 +752,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -754,7 +760,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -771,17 +777,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.125" customWidth="1"/>
-    <col min="3" max="3" width="20.875" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -792,7 +798,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>123</v>
       </c>
@@ -803,7 +809,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>456</v>
       </c>
@@ -821,19 +827,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -843,8 +850,11 @@
       <c r="C1" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -854,8 +864,11 @@
       <c r="C2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -865,16 +878,22 @@
       <c r="C3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -884,8 +903,11 @@
       <c r="C5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -894,6 +916,9 @@
       </c>
       <c r="C6" t="s">
         <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -910,13 +935,13 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.75" customWidth="1"/>
-    <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -927,7 +952,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -938,7 +963,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -949,7 +974,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -957,7 +982,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
Finished initial Crm many-to-many target
</commit_message>
<xml_diff>
--- a/IntegrationTool.UnitTests.Sources/TestData/LoadFromExcel/TestData.xlsx
+++ b/IntegrationTool.UnitTests.Sources/TestData/LoadFromExcel/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14250" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14250" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="Incidents" sheetId="6" r:id="rId4"/>
     <sheet name="Accounts" sheetId="2" r:id="rId5"/>
     <sheet name="Activities" sheetId="3" r:id="rId6"/>
+    <sheet name="Invoices" sheetId="7" r:id="rId7"/>
+    <sheet name="InvoiceContacts" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="59">
   <si>
     <t>Firstname</t>
   </si>
@@ -182,6 +184,30 @@
   </si>
   <si>
     <t>CD723ABA-3C05-E411-89D3-000C29571E8B</t>
+  </si>
+  <si>
+    <t>Invoice Number</t>
+  </si>
+  <si>
+    <t>Inv 1</t>
+  </si>
+  <si>
+    <t>Inv 2</t>
+  </si>
+  <si>
+    <t>Invoice</t>
+  </si>
+  <si>
+    <t>Invoice 1</t>
+  </si>
+  <si>
+    <t>Invoice 2</t>
+  </si>
+  <si>
+    <t>InvoiceNo</t>
+  </si>
+  <si>
+    <t>ContactID</t>
   </si>
 </sst>
 </file>
@@ -829,7 +855,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -996,4 +1022,86 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Improved loghandling of Write To Dynamics CRM target (logs now filterable)
</commit_message>
<xml_diff>
--- a/IntegrationTool.UnitTests.Sources/TestData/LoadFromExcel/TestData.xlsx
+++ b/IntegrationTool.UnitTests.Sources/TestData/LoadFromExcel/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14250" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14250"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="61">
   <si>
     <t>Firstname</t>
   </si>
@@ -208,6 +208,12 @@
   </si>
   <si>
     <t>ContactID</t>
+  </si>
+  <si>
+    <t>James again</t>
+  </si>
+  <si>
+    <t>Peter again</t>
   </si>
 </sst>
 </file>
@@ -535,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,6 +653,46 @@
       </c>
       <c r="B6" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="2">
+        <v>32843</v>
       </c>
     </row>
   </sheetData>
@@ -1068,7 +1114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>